<commit_message>
archivo de programa para práctica V
</commit_message>
<xml_diff>
--- a/clases_2025_1/documentos_actas/parejas_practica_v.xlsx
+++ b/clases_2025_1/documentos_actas/parejas_practica_v.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Grupo_1</t>
   </si>
@@ -1060,7 +1060,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -1134,7 +1134,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1143,6 +1143,9 @@
       </c>
       <c r="C7" t="s">
         <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3">

</xml_diff>